<commit_message>
Updated docu builder, more flexible
</commit_message>
<xml_diff>
--- a/Books.xlsx
+++ b/Books.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zur Bonsen Georg\Documents\Programme\Beyond4P\B4P_Docu_Maker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EA2373-A13F-4E8B-936A-F49819566C43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F168BE02-3FA4-466E-897F-DDCAFAB7389F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{3D6CAE77-ACA1-4461-B4A1-0A0F37C8EA4B}"/>
   </bookViews>
@@ -479,7 +479,7 @@
   <dimension ref="B1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Build_Docu.b4p skips include(...Library) statements
</commit_message>
<xml_diff>
--- a/Books.xlsx
+++ b/Books.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zur Bonsen Georg\Documents\Programme\Beyond4P\B4P_Docu_Maker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4274F2-64C5-487B-AE0A-36749A38E3E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F7D15F-978B-43C9-B0CF-13AEB787A74E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{3D6CAE77-ACA1-4461-B4A1-0A0F37C8EA4B}"/>
   </bookViews>
@@ -113,7 +113,7 @@
     <t>Inputs_Guide\*.txt</t>
   </si>
   <si>
-    <t>C:\Users\Zur Bonsen Georg\source\repos\Beyond4P_Code\F010*.cpp</t>
+    <t>C:\Users\Zur Bonsen Georg\source\repos\Beyond4P_Code\F0*.cpp</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Update for Rel 11.00
</commit_message>
<xml_diff>
--- a/Books.xlsx
+++ b/Books.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5444515566c7376a/Documents/Programme/Beyond4P/B4P_Docu_Maker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{B8246BD0-AB28-B246-8A82-ED27F370C745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5C3772A-B699-4E70-8C47-C04D6418529D}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{B8246BD0-AB28-B246-8A82-ED27F370C745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A576DE3F-9328-43DF-8AF8-8ADA65B070C8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3D6CAE77-ACA1-4461-B4A1-0A0F37C8EA4B}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>Book Title</t>
   </si>
@@ -98,9 +98,6 @@
     <t>LAN</t>
   </si>
   <si>
-    <t>Function Library Guide</t>
-  </si>
-  <si>
     <t>Main TOC Order</t>
   </si>
   <si>
@@ -125,13 +122,25 @@
     <t>C:/Users/zur-b/OneDrive/Documents/Programme/georgzurbonsen.github.io/</t>
   </si>
   <si>
-    <t>B4P Language</t>
-  </si>
-  <si>
     <t>Introduction</t>
   </si>
   <si>
     <t>User Guide</t>
+  </si>
+  <si>
+    <t>TAB</t>
+  </si>
+  <si>
+    <t>Inputs_Tables\*.txt</t>
+  </si>
+  <si>
+    <t>Function Library</t>
+  </si>
+  <si>
+    <t>Language Guide</t>
+  </si>
+  <si>
+    <t>Table Processing</t>
   </si>
 </sst>
 </file>
@@ -221,9 +230,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -261,7 +270,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -367,7 +376,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -509,7 +518,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -517,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B7C470-6B5E-4007-81C9-49EE72D9A7A6}">
-  <dimension ref="B1:H15"/>
+  <dimension ref="B1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +551,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -559,7 +568,7 @@
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -575,146 +584,170 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D4" s="10">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E4" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D6" s="10">
         <v>3</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E6" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="10">
+      <c r="E7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="10">
         <v>4</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E8" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="10">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
         <v>28</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H9" t="s">
+      <c r="F16" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" t="s">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E11" s="8" t="s">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="H18" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>